<commit_message>
changes made to repo
</commit_message>
<xml_diff>
--- a/activity/user_product_data.xlsx
+++ b/activity/user_product_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55" count="55">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53" count="53">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -25,160 +25,154 @@
     <x:t>productlink</x:t>
   </x:si>
   <x:si>
-    <x:t>Men Tapered Fit Chinos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 635</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/highlander/highlander-men-grey-tapered-fit-solid-chinos/2290040/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Slim Fit Chinos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 1299</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/herenow/herenow-men-grey-slim-fit-solid-chinos/9089099/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 797</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/us-polo-assn/us-polo-assn-men-khaki-slim-fit-solid-chinos/1966990/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Regular Fit Formal Trousers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 791</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/us-polo-assn/us-polo-assn-men-black-regular-fit-solid-cotton-formal-trousers/13355306/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Slim Fit Denim Joggers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 892</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/campus-sutra/campus-sutra-men-blue-slim-fit-faded-denim-joggers/13489388/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rohit Sharma Slim Fit Chinos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 696</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/highlander/highlander-by-rohit-sharma-men-navy-blue-slim-fit-checked-chinos/8375547/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/herenow/herenow-men-blue-slim-fit-solid-chinos/9064287/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 697</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/highlander/highlander-men-olive-green-tapered-fit-solid-chinos/2290044/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Regular Fit Cargos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 1399</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/roadster/roadster-men-grey-regular-fit-solid-cargos/5415202/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Slim Fit Joggers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 755</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/ivoc/ivoc-men-olive-green--black-slim-fit-printed-joggers/5333629/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Time Travlr Slim Fit Chinos</x:t>
+    <x:t>Men Printed Nehru Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 1159</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/hangup/hangup-men-beige-printed-nehru-jacket/2458630/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Solid Denim Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 730</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/jackets/locomotive/locomotive-men-blue-solid-denim-jacket/13887262/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Men Embroidered Nehru Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 1396</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/sojanya/sojanya-men-navy-blue--golden-embroidered-nehru-jacket/11562634/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Washed Denim Jacket</x:t>
   </x:si>
   <x:si>
     <x:t>Rs. 799</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.myntra.com/trousers/roadster/roadster-time-travlr-men-navy-blue-slim-fit-solid-chinos/2290971/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Regular Fit Regular Trousers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 4499</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/gant/gant-men-khaki-regular-fit-solid-regular-trousers/12539562/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Austin Trim Fit Trousers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 1494</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/us-polo-assn/us-polo-assn-men-beige-austin-trim-fit-printed-regular-trousers/13780188/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Regular Fit Chinos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 399</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/roadster/roadster-men-brown-regular-fit-solid-chinos/13859124/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 1349</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/herenow/herenow-men-green-slim-fit-solid-chinos/9089127/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 742</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/highlander/highlander-men-blue-slim-fit-solid-joggers/5125963/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 759</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/hancock/hancock-men-navy-blue-slim-fit-solid-chinos/13959050/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tapered Fit Solid Chinos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 4249</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/gant/gant-men-khaki-brown-tapered-fit-solid-chinos/13617992/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Work Essential Trousers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/invictus/invictus-men-navy-blue-solid-slim-fit-work-essential-trousers/1570784/buy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Men Regular Fit Joggers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rs. 949</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.myntra.com/trousers/roadster/roadster-men-green-regular-fit-solid-joggers/1923646/buy</x:t>
+    <x:t>https://www.myntra.com/jackets/roadster/roadster-men-blue-washed-denim-jacket/12288754/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Men Denim Sustainable Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 1749</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/jackets/hm/hm-men-black-solid-denim-sustainable-jacket/11472574/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Printed Nehru Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 702</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/maxence/maxence-men-maroon--white-floral-printed-nehru-jacket/13888034/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/jackets/highlander/highlander-men-grey-solid-denim-jacket/13665192/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Men Woven Design Nehru Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 2699</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/hangup/hangup-men-beige-woven-design-nehru-jacket/13166552/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Men Nehru Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 1229</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/kisah/kisah-men-green-woven-design-nehru-jacket/9872281/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Men Solid Denim Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 1436</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/jackets/ecko-unltd/ecko-unltd-men-solid-denim-jacket/11002856/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nehru Jacket &amp; Pocket Square</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/deyann/deyann-men-grey-printed-nehru-jacket--pocket-square/8473637/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Printed Waist Coat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 839</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/hangup/hangup-men-pink-printed-waist-coat/2447789/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Men Solid Bomber Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/jackets/dillinger/dillinger-men-maroon-solid-bomber-jacket/10986124/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 6499</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/hangup/hangup-men-pink-printed-waist-coat/2447782/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Solid Tailored Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 874</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/jackets/nautica/nautica-men-black-solid-water-resistant-tailored-jacket/13077954/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/jackets/locomotive/locomotive-men-khaki-solid-denim-jacket/13845212/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Printed Denim Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/jackets/highlander/highlander-men-blue-printed-denim-jacket/13494996/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Men Shirt Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 798</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/jackets/hm/hm-men-brown-solid-shirt-jacket/13964860/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rs. 1109</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/deyann/deyann-men-white-printed-nehru-jacket/8473593/buy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Men Solid Woven Nehru Jacket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.myntra.com/nehru-jackets/bewakoof/bewakoof-men-yellow-solid-woven-nehru-jacket/14061820/buy</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -576,46 +570,46 @@
     </x:row>
     <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
@@ -623,73 +617,73 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
       <x:c r="A12" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="A13" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
       <x:c r="A14" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
         <x:v>37</x:v>
@@ -697,18 +691,18 @@
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="A15" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="B15" s="0" t="s">
+      <x:c r="C15" s="0" t="s">
         <x:v>39</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
         <x:v>41</x:v>
@@ -719,57 +713,57 @@
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="A17" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
         <x:v>43</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
         <x:v>45</x:v>
-      </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="B19" s="0" t="s">
+      <x:c r="C19" s="0" t="s">
         <x:v>48</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="A20" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
         <x:v>50</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="C20" s="0" t="s">
-        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
         <x:v>52</x:v>
-      </x:c>
-      <x:c r="B21" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>54</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>